<commit_message>
234 quick progress, think i solved it just needs implementation
</commit_message>
<xml_diff>
--- a/234. Palindrome Linked List/Whiteboards/Solution.xlsx
+++ b/234. Palindrome Linked List/Whiteboards/Solution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\234. Palindrome Linked List\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DE802-9519-4608-B352-D1C1ED0E8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E18B05-D1A7-4457-AE53-DB5DB31FCE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -45,12 +77,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,9 +103,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -384,17 +425,718 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="K7:AX61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AL10" sqref="AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3</v>
+      </c>
+      <c r="O7" s="2">
+        <v>4</v>
+      </c>
+      <c r="P7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>6</v>
+      </c>
+      <c r="R7" s="2">
+        <v>7</v>
+      </c>
+      <c r="S7" s="2">
+        <v>8</v>
+      </c>
+      <c r="T7" s="2">
+        <v>9</v>
+      </c>
+      <c r="U7" s="2">
+        <v>10</v>
+      </c>
+      <c r="V7" s="2">
+        <v>11</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>7</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>8</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>9</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>10</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>11</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>3</v>
+      </c>
+      <c r="P8" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>5</v>
+      </c>
+      <c r="R8" s="2">
+        <v>6</v>
+      </c>
+      <c r="S8" s="2">
+        <v>7</v>
+      </c>
+      <c r="T8" s="2">
+        <v>8</v>
+      </c>
+      <c r="U8" s="2">
+        <v>9</v>
+      </c>
+      <c r="V8" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>4</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>7</v>
+      </c>
+      <c r="AJ8" s="2">
+        <v>8</v>
+      </c>
+      <c r="AK8" s="2">
+        <v>9</v>
+      </c>
+      <c r="AL8" s="2">
+        <v>10</v>
+      </c>
+      <c r="AM8" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2</v>
+      </c>
+      <c r="P10" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ10" s="2"/>
+    </row>
+    <row r="11" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1">
+        <v>2</v>
+      </c>
+      <c r="O11" s="1">
+        <v>2</v>
+      </c>
+      <c r="P11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1">
+        <v>3</v>
+      </c>
+      <c r="S11" s="1">
+        <v>2</v>
+      </c>
+      <c r="T11" s="1">
+        <v>2</v>
+      </c>
+      <c r="U11" s="1">
+        <v>2</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK11" s="2"/>
+    </row>
+    <row r="12" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL12" s="2"/>
+    </row>
+    <row r="13" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM13" s="2"/>
+    </row>
+    <row r="16" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL16" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="2"/>
+    </row>
+    <row r="17" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>3</v>
+      </c>
+      <c r="N17" s="1">
+        <v>4</v>
+      </c>
+      <c r="O17" s="1">
+        <v>4</v>
+      </c>
+      <c r="P17" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>2</v>
+      </c>
+      <c r="R17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1">
+        <v>2</v>
+      </c>
+      <c r="M21" s="1">
+        <v>3</v>
+      </c>
+      <c r="N21" s="1">
+        <v>4</v>
+      </c>
+      <c r="O21" s="1">
+        <v>4</v>
+      </c>
+      <c r="P21" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL25" s="1">
+        <v>8</v>
+      </c>
+      <c r="AM25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="1">
+        <v>5</v>
+      </c>
+      <c r="AO25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP25" s="1">
+        <v>7</v>
+      </c>
+      <c r="AQ25" s="1">
+        <v>9</v>
+      </c>
+      <c r="AR25" s="1">
+        <f>SUM(AL25:AQ25)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB26" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="1">
+        <v>9</v>
+      </c>
+      <c r="AM26" s="1">
+        <v>7</v>
+      </c>
+      <c r="AN26" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO26" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ26" s="1">
+        <v>8</v>
+      </c>
+      <c r="AR26" s="1">
+        <f>SUM(AL26:AQ26)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL27" s="1">
+        <f>AL26+AL25</f>
+        <v>17</v>
+      </c>
+      <c r="AM27" s="1">
+        <f t="shared" ref="AM27:AQ27" si="0">AM26+AM25</f>
+        <v>8</v>
+      </c>
+      <c r="AN27" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AO27" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AP27" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AQ27" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ32" s="1">
+        <v>8</v>
+      </c>
+      <c r="AK32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL32" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM32" s="1">
+        <v>3</v>
+      </c>
+      <c r="AN32" s="1">
+        <v>7</v>
+      </c>
+      <c r="AO32" s="1">
+        <v>9</v>
+      </c>
+      <c r="AP32" s="1">
+        <v>9</v>
+      </c>
+      <c r="AQ32" s="1">
+        <v>7</v>
+      </c>
+      <c r="AR32" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS32" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU32" s="1">
+        <v>8</v>
+      </c>
+      <c r="AX32" s="1">
+        <f>SUM(AJ32:AU32)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="36:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ55" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK55" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL55" s="1">
+        <v>7</v>
+      </c>
+      <c r="AM55" s="1">
+        <v>7</v>
+      </c>
+      <c r="AN55" s="1">
+        <v>6</v>
+      </c>
+      <c r="AO55" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP55" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ55" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR55" s="2">
+        <v>7</v>
+      </c>
+      <c r="AS55" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT55" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="36:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ60" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK60" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL60" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="36:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ61" s="1">
+        <v>7</v>
+      </c>
+      <c r="AK61" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
slow progress on 234 with modified constraints
</commit_message>
<xml_diff>
--- a/234. Palindrome Linked List/Whiteboards/Solution.xlsx
+++ b/234. Palindrome Linked List/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\234. Palindrome Linked List\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E18B05-D1A7-4457-AE53-DB5DB31FCE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A430DA9E-02A8-48C2-905C-1B409AABA3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>&gt;</t>
   </si>
@@ -63,6 +63,15 @@
   <si>
     <t>L8</t>
   </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>hol</t>
+  </si>
 </sst>
 </file>
 
@@ -77,7 +86,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +96,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -103,12 +124,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -425,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="K7:AX61"/>
+  <dimension ref="K6:AX61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AL10" sqref="AL10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -436,7 +463,18 @@
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP6" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L7" s="2">
         <v>1</v>
       </c>
@@ -506,8 +544,20 @@
       <c r="AM7" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="4">
+        <v>2</v>
+      </c>
+      <c r="AR7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AS7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L8" s="2">
         <v>0</v>
       </c>
@@ -577,8 +627,23 @@
       <c r="AM8" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="4">
+        <v>2</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS8" s="3">
+        <v>2</v>
+      </c>
+      <c r="AT8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB9" s="1">
         <v>1</v>
       </c>
@@ -615,8 +680,26 @@
       <c r="AM9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR9" s="4">
+        <v>3</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>3</v>
+      </c>
+      <c r="AT9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AU9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L10" s="1">
         <v>1</v>
       </c>
@@ -643,7 +726,7 @@
       </c>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L11" s="1">
         <v>1</v>
       </c>
@@ -703,7 +786,7 @@
       </c>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB12" s="1">
         <v>6</v>
       </c>
@@ -730,7 +813,7 @@
       </c>
       <c r="AL12" s="2"/>
     </row>
-    <row r="13" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AK13" s="2">
         <v>3</v>
       </c>
@@ -739,7 +822,18 @@
       </c>
       <c r="AM13" s="2"/>
     </row>
-    <row r="16" spans="12:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="12:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AL16" s="2">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
forgot to ctrl+S these notes
</commit_message>
<xml_diff>
--- a/234. Palindrome Linked List/Whiteboards/Solution.xlsx
+++ b/234. Palindrome Linked List/Whiteboards/Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\234. Palindrome Linked List\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A430DA9E-02A8-48C2-905C-1B409AABA3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507DDA5A-4239-4EFB-B00A-FACFE3814334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>&gt;</t>
   </si>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="K6:AX61"/>
+  <dimension ref="F6:AX61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="AN16" s="2"/>
     </row>
-    <row r="17" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K17" s="1">
         <v>1</v>
       </c>
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K18" s="1" t="s">
         <v>8</v>
       </c>
@@ -912,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AC19" s="1">
         <v>3</v>
       </c>
@@ -923,12 +923,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K21" s="1">
         <v>1</v>
       </c>
@@ -954,7 +954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K22" s="1" t="s">
         <v>8</v>
       </c>
@@ -980,7 +980,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1">
+        <v>4</v>
+      </c>
+      <c r="J24" s="1">
+        <v>5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>6</v>
+      </c>
+      <c r="L24" s="1">
+        <v>7</v>
+      </c>
+      <c r="M24" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB25" s="1">
         <v>1</v>
       </c>
@@ -1022,7 +1048,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="AB26" s="1">
         <v>6</v>
       </c>
@@ -1064,7 +1099,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="1">
+        <v>5</v>
+      </c>
+      <c r="K27" s="1">
+        <v>6</v>
+      </c>
+      <c r="L27" s="1">
+        <v>7</v>
+      </c>
       <c r="AL27" s="1">
         <f>AL26+AL25</f>
         <v>17</v>
@@ -1090,7 +1134,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="1">
+        <v>6</v>
+      </c>
+      <c r="L28" s="1">
+        <v>7</v>
+      </c>
+      <c r="M28" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AJ31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="11:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AJ32" s="1">
         <v>8</v>
       </c>

</xml_diff>